<commit_message>
dat hang -> ban hang
</commit_message>
<xml_diff>
--- a/public/backend/file/product_custom_import_export.xlsx
+++ b/public/backend/file/product_custom_import_export.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>quantity</t>
   </si>
@@ -38,28 +38,19 @@
     <t>serials</t>
   </si>
   <si>
-    <t>mới</t>
-  </si>
-  <si>
     <t>SG</t>
   </si>
   <si>
-    <t>code</t>
-  </si>
-  <si>
-    <t>diameter</t>
-  </si>
-  <si>
-    <t>category</t>
-  </si>
-  <si>
-    <t>B05</t>
-  </si>
-  <si>
-    <t>Standard</t>
-  </si>
-  <si>
     <t>12-33-21</t>
+  </si>
+  <si>
+    <t>name</t>
+  </si>
+  <si>
+    <t>B05-11.4-Standard</t>
+  </si>
+  <si>
+    <t>Mới</t>
   </si>
 </sst>
 </file>
@@ -391,67 +382,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G2" sqref="G2"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="6.109375" customWidth="1"/>
-    <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="10.5546875" customWidth="1"/>
-    <col min="4" max="4" width="7.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.44140625" customWidth="1"/>
-    <col min="6" max="6" width="11.109375" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="16.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.44140625" customWidth="1"/>
+    <col min="4" max="4" width="11.109375" customWidth="1"/>
+    <col min="5" max="5" width="16.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
         <v>7</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>2</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B2">
-        <v>11.4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>10</v>
-      </c>
-      <c r="D2">
+      <c r="D2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" t="s">
         <v>5</v>
-      </c>
-      <c r="E2" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" t="s">
-        <v>5</v>
-      </c>
-      <c r="G2" t="s">
-        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>